<commit_message>
Init jira aiotest manager
</commit_message>
<xml_diff>
--- a/src/test/data/SauceDemo.xlsx
+++ b/src/test/data/SauceDemo.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\PlaywrightCucumber\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E13392A3-0D4B-4F86-A92B-FF62623C4CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F9D051-189C-49A9-9048-65816FB539C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E2AC2319-EE85-4FFD-83F6-F706E8CA498A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E2AC2319-EE85-4FFD-83F6-F706E8CA498A}"/>
   </bookViews>
   <sheets>
     <sheet name="HomePage" sheetId="1" r:id="rId1"/>
-    <sheet name="InventoryPage" sheetId="2" r:id="rId2"/>
+    <sheet name="info" sheetId="3" r:id="rId2"/>
+    <sheet name="InventoryPage" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="HomePage" localSheetId="0">info!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>pageName</t>
   </si>
@@ -53,13 +57,34 @@
   </si>
   <si>
     <t>#login-button</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>InventoryPage</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/inventory.html</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>.shopping_cart_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +103,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -123,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -133,6 +164,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -451,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534AB0A2-AF9B-4F9E-BB4E-C52A1EC1F85D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,13 +545,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261434C2-4521-4505-BFA9-DD6AD95112F9}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F2E8E5-DE25-41DE-9A83-A27885F446C1}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" style="1" customWidth="1"/>
+    <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261434C2-4521-4505-BFA9-DD6AD95112F9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish converting from excel to pom
</commit_message>
<xml_diff>
--- a/src/test/data/SauceDemo.xlsx
+++ b/src/test/data/SauceDemo.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\PlaywrightCucumber\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F9D051-189C-49A9-9048-65816FB539C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF9CD4D-8EF5-4A5E-9F31-93512C6F1B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E2AC2319-EE85-4FFD-83F6-F706E8CA498A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E2AC2319-EE85-4FFD-83F6-F706E8CA498A}"/>
   </bookViews>
   <sheets>
-    <sheet name="HomePage" sheetId="1" r:id="rId1"/>
-    <sheet name="info" sheetId="3" r:id="rId2"/>
+    <sheet name="info" sheetId="3" r:id="rId1"/>
+    <sheet name="HomePage" sheetId="1" r:id="rId2"/>
     <sheet name="InventoryPage" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="HomePage" localSheetId="0">info!$A$2</definedName>
+    <definedName name="HomePage" localSheetId="1">info!$A$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>pageName</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>.shopping_cart_link</t>
+  </si>
+  <si>
+    <t>element</t>
   </si>
 </sst>
 </file>
@@ -488,67 +491,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534AB0A2-AF9B-4F9E-BB4E-C52A1EC1F85D}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F2E8E5-DE25-41DE-9A83-A27885F446C1}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -588,13 +534,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534AB0A2-AF9B-4F9E-BB4E-C52A1EC1F85D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261434C2-4521-4505-BFA9-DD6AD95112F9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -604,7 +603,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>

</xml_diff>